<commit_message>
Added walkthrough, updated project2 page with embed link and fixed project1 link
</commit_message>
<xml_diff>
--- a/projects/dataProject2/Operations_Tracker_Dataset.xlsx
+++ b/projects/dataProject2/Operations_Tracker_Dataset.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SusanSensemanWebsite\projects\dataProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE647E-AF0C-4428-9D2F-FAE5609C3C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F774B-8CE3-404A-AD86-CD27573C6B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23460" yWindow="555" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -521,13 +522,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="I181" sqref="I181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -585,7 +596,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -614,7 +625,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -643,7 +654,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -672,7 +683,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -701,7 +712,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -730,7 +741,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -759,7 +770,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -788,7 +799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -817,7 +828,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -846,7 +857,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -875,7 +886,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -904,7 +915,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -933,7 +944,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -962,7 +973,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -991,7 +1002,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1031,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1049,7 +1060,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1078,7 +1089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1107,7 +1118,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1136,7 +1147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1176,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1205,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1234,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1252,7 +1263,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1292,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1339,7 +1350,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1368,7 +1379,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1397,7 +1408,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1466,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1495,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1513,7 +1524,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1542,7 +1553,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1571,7 +1582,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1600,7 +1611,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1658,7 +1669,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1687,7 +1698,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1727,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1745,7 +1756,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1774,7 +1785,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1814,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1832,7 +1843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -1861,7 +1872,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +1901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -1919,7 +1930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -1948,7 +1959,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -1977,7 +1988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2006,7 +2017,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2035,7 +2046,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2064,7 +2075,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2093,7 +2104,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2122,7 +2133,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -2151,7 +2162,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2180,7 +2191,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -2209,7 +2220,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -2238,7 +2249,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -2267,7 +2278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -2354,7 +2365,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -2383,7 +2394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -2412,7 +2423,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2441,7 +2452,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -2470,7 +2481,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2499,7 +2510,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2528,7 +2539,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2586,7 +2597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2615,7 +2626,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2644,7 +2655,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -2702,7 +2713,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -2731,7 +2742,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>20</v>
       </c>
@@ -2760,7 +2771,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -2789,7 +2800,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>20</v>
       </c>
@@ -2818,7 +2829,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>21</v>
       </c>
@@ -2847,7 +2858,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>21</v>
       </c>
@@ -2876,7 +2887,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -2905,7 +2916,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>21</v>
       </c>
@@ -2934,7 +2945,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>21</v>
       </c>
@@ -2963,7 +2974,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>21</v>
       </c>
@@ -2992,7 +3003,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -3021,7 +3032,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -3050,7 +3061,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -3079,7 +3090,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -3108,7 +3119,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -3137,7 +3148,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -3166,7 +3177,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -3195,7 +3206,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -3224,7 +3235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>23</v>
       </c>
@@ -3253,7 +3264,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -3282,7 +3293,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>23</v>
       </c>
@@ -3311,7 +3322,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>23</v>
       </c>
@@ -3340,7 +3351,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>24</v>
       </c>
@@ -3369,7 +3380,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -3398,7 +3409,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>24</v>
       </c>
@@ -3427,7 +3438,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -3456,7 +3467,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
@@ -3485,7 +3496,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -3514,7 +3525,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -3543,7 +3554,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>25</v>
       </c>
@@ -3572,7 +3583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>25</v>
       </c>
@@ -3601,7 +3612,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>25</v>
       </c>
@@ -3630,7 +3641,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -3659,7 +3670,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>25</v>
       </c>
@@ -3688,7 +3699,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>26</v>
       </c>
@@ -3717,7 +3728,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -3746,7 +3757,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>26</v>
       </c>
@@ -3775,7 +3786,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -3804,7 +3815,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>26</v>
       </c>
@@ -3833,7 +3844,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -3862,7 +3873,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3902,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -3920,7 +3931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>27</v>
       </c>
@@ -3949,7 +3960,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>27</v>
       </c>
@@ -3978,7 +3989,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>27</v>
       </c>
@@ -4007,7 +4018,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>27</v>
       </c>
@@ -4036,7 +4047,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>28</v>
       </c>
@@ -4065,7 +4076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>28</v>
       </c>
@@ -4094,7 +4105,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>28</v>
       </c>
@@ -4123,7 +4134,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -4152,7 +4163,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>28</v>
       </c>
@@ -4181,7 +4192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>28</v>
       </c>
@@ -4210,7 +4221,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>29</v>
       </c>
@@ -4239,7 +4250,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>29</v>
       </c>
@@ -4268,7 +4279,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>29</v>
       </c>
@@ -4297,7 +4308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>29</v>
       </c>
@@ -4326,7 +4337,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>29</v>
       </c>
@@ -4355,7 +4366,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>29</v>
       </c>
@@ -4384,7 +4395,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -4413,7 +4424,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>30</v>
       </c>
@@ -4442,7 +4453,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -4471,7 +4482,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>30</v>
       </c>
@@ -4500,7 +4511,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -4529,7 +4540,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>30</v>
       </c>
@@ -4558,7 +4569,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>31</v>
       </c>
@@ -4587,7 +4598,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>31</v>
       </c>
@@ -4616,7 +4627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>31</v>
       </c>
@@ -4645,7 +4656,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>31</v>
       </c>
@@ -4674,7 +4685,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>31</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -4732,7 +4743,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>32</v>
       </c>
@@ -4761,7 +4772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>32</v>
       </c>
@@ -4790,7 +4801,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>32</v>
       </c>
@@ -4819,7 +4830,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -4848,7 +4859,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>32</v>
       </c>
@@ -4877,7 +4888,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>32</v>
       </c>
@@ -4906,7 +4917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>33</v>
       </c>
@@ -4935,7 +4946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>33</v>
       </c>
@@ -4964,7 +4975,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>33</v>
       </c>
@@ -4993,7 +5004,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>33</v>
       </c>
@@ -5022,7 +5033,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>33</v>
       </c>
@@ -5051,7 +5062,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>33</v>
       </c>
@@ -5080,7 +5091,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>34</v>
       </c>
@@ -5109,7 +5120,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>34</v>
       </c>
@@ -5138,7 +5149,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>34</v>
       </c>
@@ -5167,7 +5178,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>34</v>
       </c>
@@ -5196,7 +5207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>34</v>
       </c>
@@ -5225,7 +5236,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>34</v>
       </c>
@@ -5254,7 +5265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>35</v>
       </c>
@@ -5283,7 +5294,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>35</v>
       </c>
@@ -5312,7 +5323,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>35</v>
       </c>
@@ -5341,7 +5352,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -5399,7 +5410,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>35</v>
       </c>
@@ -5428,7 +5439,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -5457,7 +5468,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -5486,7 +5497,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>36</v>
       </c>
@@ -5515,7 +5526,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>36</v>
       </c>
@@ -5544,7 +5555,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>36</v>
       </c>
@@ -5573,7 +5584,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>36</v>
       </c>
@@ -5602,7 +5613,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>37</v>
       </c>
@@ -5631,7 +5642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>37</v>
       </c>
@@ -5660,7 +5671,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>37</v>
       </c>
@@ -5689,7 +5700,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>37</v>
       </c>
@@ -5718,7 +5729,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>37</v>
       </c>
@@ -5747,7 +5758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>37</v>
       </c>
@@ -5773,6 +5784,24 @@
         <v>88</v>
       </c>
       <c r="I181">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7BBB57-0999-4720-A9BD-5D99EF6E1BDA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>83</v>
       </c>
     </row>

</xml_diff>